<commit_message>
Added options for categories and pages 1. Added field to select from which category the products will be exported 2. Added field to select which pages should be exported (only products, only association, both)
</commit_message>
<xml_diff>
--- a/Example Sheet.xlsx
+++ b/Example Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20374"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Área de Trabalho\Matheus\Github\Export Magento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4A8782-142E-4D29-BDE2-186CE4C9E8C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FCC133-E41A-4148-BC06-A97F26BFDBBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t>store</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Configurable Product Short Description</t>
   </si>
   <si>
-    <t>2021-05-15T17:55:21-03:00</t>
-  </si>
-  <si>
     <t>simple</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>Configurable Product-G</t>
   </si>
   <si>
-    <t>2021-05-15T17:56:10-03:00</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>Configurable Product-M</t>
   </si>
   <si>
-    <t>2021-05-15T17:56:19-03:00</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -155,9 +146,6 @@
     <t>Configurable Product-P</t>
   </si>
   <si>
-    <t>2021-05-15T17:56:28-03:00</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -173,9 +161,6 @@
     <t>Simple Product Short Description</t>
   </si>
   <si>
-    <t>2021-05-15T17:57:34-03:00</t>
-  </si>
-  <si>
     <t>Yellow</t>
   </si>
   <si>
@@ -188,9 +173,6 @@
     <t>Produto Teste</t>
   </si>
   <si>
-    <t>2021-05-16T13:19:14-03:00</t>
-  </si>
-  <si>
     <t>_super_products_sku</t>
   </si>
   <si>
@@ -204,6 +186,12 @@
   </si>
   <si>
     <t>Short Desc</t>
+  </si>
+  <si>
+    <t>2021-05-15</t>
+  </si>
+  <si>
+    <t>2021-05-16</t>
   </si>
 </sst>
 </file>
@@ -237,8 +225,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,12 +535,12 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="23.7109375" customWidth="1"/>
+    <col min="19" max="19" width="23.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -609,7 +598,7 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" t="s">
@@ -674,8 +663,8 @@
       <c r="R2">
         <v>0</v>
       </c>
-      <c r="S2" t="s">
-        <v>32</v>
+      <c r="S2" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -689,16 +678,16 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
       </c>
       <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
         <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -733,11 +722,11 @@
       <c r="R3">
         <v>0</v>
       </c>
-      <c r="S3" t="s">
-        <v>36</v>
+      <c r="S3" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="U3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -751,16 +740,16 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4">
         <v>100</v>
@@ -795,11 +784,11 @@
       <c r="R4">
         <v>0</v>
       </c>
-      <c r="S4" t="s">
-        <v>40</v>
+      <c r="S4" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="U4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -813,16 +802,16 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H5">
         <v>100</v>
@@ -857,11 +846,11 @@
       <c r="R5">
         <v>0</v>
       </c>
-      <c r="S5" t="s">
-        <v>44</v>
+      <c r="S5" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="U5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -875,16 +864,16 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>20</v>
@@ -905,10 +894,10 @@
         <v>29</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -919,14 +908,14 @@
       <c r="R6">
         <v>0</v>
       </c>
-      <c r="S6" t="s">
-        <v>50</v>
+      <c r="S6" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="T6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="V6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -940,13 +929,13 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H7">
         <v>40</v>
@@ -967,10 +956,10 @@
         <v>29</v>
       </c>
       <c r="N7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="O7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -981,8 +970,8 @@
       <c r="R7">
         <v>0</v>
       </c>
-      <c r="S7" t="s">
-        <v>55</v>
+      <c r="S7" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1004,13 +993,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,35 +1012,35 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>